<commit_message>
fin cours 22 fev, cas de test et scénario sur camisoles inventaires objets et shorts
</commit_message>
<xml_diff>
--- a/Requis_Remise/Tests.xlsx
+++ b/Requis_Remise/Tests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Liste inventaires (205)" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="222">
   <si>
     <t>Test sur la création d'utilisateur</t>
   </si>
@@ -644,13 +644,71 @@
     <t>Objet-Msg-03</t>
   </si>
   <si>
-    <t>Veuillez entrer la description de l'objet</t>
-  </si>
-  <si>
     <t>Veuillez entrer la couleur de l'objet</t>
   </si>
   <si>
     <t>Veuillez entrer la quantité de l'objet</t>
+  </si>
+  <si>
+    <t>Veuillez entrer le nom de l'objet</t>
+  </si>
+  <si>
+    <t>Objet --&gt; Rien saisir</t>
+  </si>
+  <si>
+    <t>Objet --&gt; Cône</t>
+  </si>
+  <si>
+    <t>Couleur --&gt; Orange</t>
+  </si>
+  <si>
+    <t>Quantité --&gt; 10000</t>
+  </si>
+  <si>
+    <t>T-Inventaire-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantité --&gt;abc </t>
+  </si>
+  <si>
+    <t>La quantité de short ne peut pas être inférieur que la quantité empruntée</t>
+  </si>
+  <si>
+    <t>Short-Msg-06</t>
+  </si>
+  <si>
+    <t>Quantité --&gt; Rien entrer</t>
+  </si>
+  <si>
+    <t>T-Inventaire-8</t>
+  </si>
+  <si>
+    <t>Objet-Msg-04</t>
+  </si>
+  <si>
+    <t>Seulement les nombres sont acceptés</t>
+  </si>
+  <si>
+    <t>Objet-Msg-05</t>
+  </si>
+  <si>
+    <t>Short-Msg-07</t>
+  </si>
+  <si>
+    <t>Objet-Msg-04
+Objet-Msg-05</t>
+  </si>
+  <si>
+    <t>Quantité accepté</t>
+  </si>
+  <si>
+    <t>Le champs limite le nombre à 4 chiffres</t>
+  </si>
+  <si>
+    <t>Couleur acceptée</t>
+  </si>
+  <si>
+    <t>Nom de l'objet accepté</t>
   </si>
 </sst>
 </file>
@@ -686,7 +744,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -825,11 +883,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -844,18 +911,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -878,15 +933,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -898,6 +944,32 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1097,13 +1169,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1113,6 +1178,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1138,6 +1210,104 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1233,13 +1403,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1249,6 +1412,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1350,13 +1520,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1366,6 +1529,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1391,35 +1561,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1496,13 +1637,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1512,6 +1646,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1537,6 +1678,104 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1593,6 +1832,9 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1600,9 +1842,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1628,72 +1867,16 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1703,23 +1886,10 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1742,104 +1912,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -1856,24 +1928,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau8" displayName="Tableau8" ref="A4:D14" totalsRowShown="0" headerRowDxfId="32" dataDxfId="33" headerRowBorderDxfId="38" tableBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau8" displayName="Tableau8" ref="A4:D14" totalsRowShown="0" headerRowDxfId="68" dataDxfId="66" headerRowBorderDxfId="67" tableBorderDxfId="65">
   <autoFilter ref="A4:D14"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Numéro (No_Page)" dataDxfId="37"/>
-    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="36"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="35"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="34"/>
+    <tableColumn id="1" name="Numéro (No_Page)" dataDxfId="64"/>
+    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="63"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="62"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A23:D44" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="51" tableBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A23:D44" totalsRowShown="0" headerRowDxfId="60" headerRowBorderDxfId="59" tableBorderDxfId="58">
   <autoFilter ref="A23:D44"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Numéro " dataDxfId="50"/>
-    <tableColumn id="2" name="Manipulations" dataDxfId="49"/>
+    <tableColumn id="1" name="Numéro " dataDxfId="57"/>
+    <tableColumn id="2" name="Manipulations" dataDxfId="56"/>
     <tableColumn id="3" name="Résultat attendu"/>
     <tableColumn id="4" name="Résultat obtenu"/>
   </tableColumns>
@@ -1882,8 +1954,21 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="A4:D20" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="45" tableBorderDxfId="46" totalsRowBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="A4:D20" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="A4:D20"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Numéro " dataDxfId="51"/>
+    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="50"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="49"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="48"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A4:D10" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+  <autoFilter ref="A4:D10"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Numéro " dataDxfId="43"/>
     <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="42"/>
@@ -1894,48 +1979,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A4:D10" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="67" tableBorderDxfId="68" totalsRowBorderDxfId="66">
-  <autoFilter ref="A4:D10"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Numéro " dataDxfId="65"/>
-    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="64"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="63"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="62"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A13:D27" totalsRowShown="0" headerRowDxfId="53" headerRowBorderDxfId="59" tableBorderDxfId="60" totalsRowBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A13:D27" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
   <autoFilter ref="A13:D27"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Numéro " dataDxfId="57"/>
-    <tableColumn id="2" name="Manipulations" dataDxfId="56"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="55"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="54"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tableau312" displayName="Tableau312" ref="A4:D10" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="13" tableBorderDxfId="14" totalsRowBorderDxfId="12">
-  <autoFilter ref="A4:D10"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Numéro " dataDxfId="11"/>
-    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="10"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="9"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="8"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tableau413" displayName="Tableau413" ref="A13:D17" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
-  <autoFilter ref="A13:D17"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Numéro " dataDxfId="3"/>
     <tableColumn id="2" name="Manipulations" dataDxfId="2"/>
@@ -1946,27 +1992,53 @@
 </table>
 </file>
 
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tableau312" displayName="Tableau312" ref="A4:D12" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+  <autoFilter ref="A4:D12"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Numéro " dataDxfId="35"/>
+    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="34"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="33"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="32"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tableau413" displayName="Tableau413" ref="A15:D19" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+  <autoFilter ref="A15:D19"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Numéro " dataDxfId="27"/>
+    <tableColumn id="2" name="Manipulations" dataDxfId="26"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="25"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="24"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tableau9" displayName="Tableau9" ref="A4:D9" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="30" tableBorderDxfId="31" totalsRowBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tableau9" displayName="Tableau9" ref="A4:D9" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
   <autoFilter ref="A4:D9"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Numéro" dataDxfId="28"/>
-    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="27"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="26"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="25"/>
+    <tableColumn id="1" name="Numéro" dataDxfId="19"/>
+    <tableColumn id="2" name="Champ Traité --&gt; Valeur" dataDxfId="18"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="17"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tableau10" displayName="Tableau10" ref="A12:D33" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="22" tableBorderDxfId="23" totalsRowBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tableau10" displayName="Tableau10" ref="A12:D33" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <autoFilter ref="A12:D33"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Numéro" dataDxfId="20"/>
-    <tableColumn id="2" name="Manipulations" dataDxfId="19"/>
-    <tableColumn id="3" name="Résultat attendu" dataDxfId="18"/>
-    <tableColumn id="4" name="Résultat obtenu" dataDxfId="17"/>
+    <tableColumn id="1" name="Numéro" dataDxfId="11"/>
+    <tableColumn id="2" name="Manipulations" dataDxfId="10"/>
+    <tableColumn id="3" name="Résultat attendu" dataDxfId="9"/>
+    <tableColumn id="4" name="Résultat obtenu" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2251,40 +2323,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="11" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2462,45 +2534,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="8" t="s">
         <v>80</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -2509,12 +2581,12 @@
       <c r="C5" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="9" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="8" t="s">
         <v>81</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -2523,12 +2595,12 @@
       <c r="C6" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="9" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="8" t="s">
         <v>82</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -2537,12 +2609,12 @@
       <c r="C7" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="9" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="8" t="s">
         <v>83</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -2551,12 +2623,12 @@
       <c r="C8" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="9" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="8" t="s">
         <v>84</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -2565,12 +2637,12 @@
       <c r="C9" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="9" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="8" t="s">
         <v>85</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2579,12 +2651,12 @@
       <c r="C10" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="9" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="8" t="s">
         <v>86</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -2593,7 +2665,7 @@
       <c r="C11" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="9" t="s">
         <v>126</v>
       </c>
       <c r="E11" t="s">
@@ -2601,7 +2673,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="8" t="s">
         <v>87</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -2610,12 +2682,12 @@
       <c r="C12" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="9" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="8" t="s">
         <v>109</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -2624,12 +2696,12 @@
       <c r="C13" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="9" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="8" t="s">
         <v>110</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -2638,12 +2710,12 @@
       <c r="C14" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="9" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="8" t="s">
         <v>111</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -2652,12 +2724,12 @@
       <c r="C15" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="9" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="8" t="s">
         <v>112</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -2666,12 +2738,12 @@
       <c r="C16" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="9" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="8" t="s">
         <v>113</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -2680,12 +2752,12 @@
       <c r="C17" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="9" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="8" t="s">
         <v>114</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -2694,12 +2766,12 @@
       <c r="C18" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="9" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="8" t="s">
         <v>115</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -2708,21 +2780,21 @@
       <c r="C19" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="9" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="15" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2733,86 +2805,86 @@
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="18" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22" t="s">
+      <c r="A25" s="18"/>
+      <c r="B25" s="18" t="s">
         <v>135</v>
       </c>
       <c r="C25" s="2"/>
-      <c r="D25" s="23"/>
+      <c r="D25" s="19"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22" t="s">
+      <c r="A26" s="18"/>
+      <c r="B26" s="18" t="s">
         <v>136</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="23"/>
+      <c r="D26" s="19"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22" t="s">
+      <c r="A27" s="18"/>
+      <c r="B27" s="18" t="s">
         <v>137</v>
       </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="23"/>
+      <c r="D27" s="19"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22" t="s">
+      <c r="A28" s="18"/>
+      <c r="B28" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="21"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="17"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="21"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="17"/>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="18" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -2821,12 +2893,12 @@
       <c r="D30" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="E30" s="21"/>
+      <c r="E30" s="17"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
@@ -2835,10 +2907,10 @@
       <c r="B32" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="D32" s="22" t="s">
+      <c r="D32" s="18" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2869,10 +2941,10 @@
       <c r="B36" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C36" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="D36" s="22" t="s">
+      <c r="D36" s="18" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2903,10 +2975,10 @@
       <c r="B40" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="D40" s="22" t="s">
+      <c r="D40" s="18" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2947,14 +3019,14 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="18"/>
-      <c r="B44" s="18" t="s">
+      <c r="A44" s="14"/>
+      <c r="B44" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="C44" s="31" t="s">
+      <c r="C44" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="D44" s="31" t="s">
+      <c r="D44" s="24" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2979,7 +3051,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2991,45 +3063,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="8" t="s">
         <v>156</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -3038,12 +3110,12 @@
       <c r="C5" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="9" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="8" t="s">
         <v>163</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -3052,12 +3124,12 @@
       <c r="C6" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="9" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="8" t="s">
         <v>164</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -3066,12 +3138,12 @@
       <c r="C7" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="9" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="8" t="s">
         <v>165</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -3080,12 +3152,12 @@
       <c r="C8" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="9" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="8" t="s">
         <v>166</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -3094,21 +3166,21 @@
       <c r="C9" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="15" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3119,174 +3191,174 @@
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="31"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="21" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="22" t="s">
+      <c r="A15" s="8"/>
+      <c r="B15" s="18" t="s">
         <v>177</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="13"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="22" t="s">
+      <c r="A16" s="8"/>
+      <c r="B16" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="22" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="13"/>
+      <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="21" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="22" t="s">
+      <c r="A19" s="8"/>
+      <c r="B19" s="18" t="s">
         <v>183</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="28"/>
+      <c r="D19" s="21"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="22" t="s">
+      <c r="A20" s="8"/>
+      <c r="B20" s="18" t="s">
         <v>184</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="13"/>
+      <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="22" t="s">
+      <c r="A21" s="8"/>
+      <c r="B21" s="18" t="s">
         <v>187</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="9" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="13"/>
+      <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="18" t="s">
         <v>176</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="9" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
+      <c r="A24" s="8"/>
       <c r="B24" s="2" t="s">
         <v>145</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="9" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
+      <c r="A25" s="8"/>
       <c r="B25" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="D25" s="30" t="s">
+      <c r="D25" s="23" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
+      <c r="A26" s="8"/>
       <c r="B26" s="2" t="s">
         <v>145</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="9" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="18" t="s">
+      <c r="A27" s="13"/>
+      <c r="B27" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="15" t="s">
         <v>189</v>
       </c>
     </row>
@@ -3307,10 +3379,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3322,185 +3394,213 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="8" t="s">
         <v>191</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>157</v>
+        <v>203</v>
+      </c>
+      <c r="C5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="8" t="s">
         <v>192</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>162</v>
+        <v>204</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>129</v>
+        <v>221</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="8" t="s">
         <v>193</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>159</v>
+        <v>119</v>
+      </c>
+      <c r="C7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D7" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="8" t="s">
         <v>194</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>169</v>
+        <v>205</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>161</v>
+        <v>220</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="8" t="s">
         <v>195</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="C10" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>217</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="35"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="13"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="31"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B15" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C15" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D15" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="28"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="13"/>
-    </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="29"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="21"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="2"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="13"/>
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="22"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -3551,45 +3651,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="8" t="s">
         <v>103</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -3598,12 +3698,12 @@
       <c r="C5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="25" t="s">
         <v>104</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -3612,12 +3712,12 @@
       <c r="C6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="26" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="8" t="s">
         <v>105</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -3626,12 +3726,12 @@
       <c r="C7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="25" t="s">
         <v>106</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -3640,48 +3740,48 @@
       <c r="C8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="26" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="15" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="8" t="s">
         <v>98</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -3690,43 +3790,43 @@
       <c r="C13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="13"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="13"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="13"/>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="23" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3737,7 +3837,7 @@
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="8" t="s">
         <v>99</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -3746,43 +3846,43 @@
       <c r="C19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="13"/>
+      <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="13"/>
+      <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="13"/>
+      <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="23" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3793,7 +3893,7 @@
       <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="8" t="s">
         <v>100</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -3802,43 +3902,43 @@
       <c r="C25" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
+      <c r="A26" s="8"/>
       <c r="B26" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="13"/>
+      <c r="D26" s="9"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
+      <c r="A27" s="8"/>
       <c r="B27" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="13"/>
+      <c r="D27" s="9"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
+      <c r="A28" s="8"/>
       <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="13"/>
+      <c r="D28" s="9"/>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
+      <c r="A29" s="8"/>
       <c r="B29" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="30" t="s">
+      <c r="D29" s="23" t="s">
         <v>79</v>
       </c>
     </row>
@@ -3849,7 +3949,7 @@
       <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="8" t="s">
         <v>101</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -3858,27 +3958,27 @@
       <c r="C31" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
+      <c r="A32" s="8"/>
       <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C32" s="2"/>
-      <c r="D32" s="13"/>
+      <c r="D32" s="9"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
-      <c r="B33" s="18" t="s">
+      <c r="A33" s="13"/>
+      <c r="B33" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="15" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3899,10 +3999,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" activeCellId="1" sqref="A25 A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3912,22 +4012,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
@@ -3938,172 +4038,214 @@
       <c r="A4" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>157</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>159</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>161</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>186</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="32" t="s">
         <v>185</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>189</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="32" t="s">
         <v>188</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
+      <c r="A18" t="s">
+        <v>210</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>197</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
+        <v>216</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>198</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>197</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>198</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>199</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
+      <c r="B23" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>213</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>215</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="17">
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B4:D4"/>
@@ -4112,13 +4254,10 @@
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>